<commit_message>
update para poner a prueba
</commit_message>
<xml_diff>
--- a/ListadoCompleto.xlsx
+++ b/ListadoCompleto.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,26 +429,6 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>chino3</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Nombre</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>chino2</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Nombre</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
           <t>chino</t>
         </is>
       </c>
@@ -464,223 +444,33 @@
           <t>CANTIDAD</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>PRODUCTO</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>CANTIDAD</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>PRODUCTO</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>CANTIDAD</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Marine boy Fried seasoning
-Snack sabor salsa frita</t>
+          <t>Zanahoria</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.5</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>PIEZAS</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Korean macaroni
-Frituras</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>PIEZAS</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>PRODUCTO 1</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>PIEZAS</t>
+          <t>KG</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Anchovy fish sauce 3kg
-Salsa de pescado anchoas</t>
+          <t>TOTAL</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.5</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>PIEZAS</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Onion rings
-Frituras sabor aros de 
-cebolla</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>PIEZAS</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>PRODUCTO1</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>0.5</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>PIEZAS</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>PRODUCTO 2</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>1.5</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>PIEZAS</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Homerun ball
-Biscochos rellenos de 
-chocolate</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>PIEZAS</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>PRODUCTO 2</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>PIEZAS</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>$ 735.0</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>$ 169.0</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Onion rings
-Frituras sabor aros de 
-cebolla</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>PIEZAS</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>$ 317.5</t>
+          <t>$ 0.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agregan los perfiles para pruebas
</commit_message>
<xml_diff>
--- a/ListadoCompleto.xlsx
+++ b/ListadoCompleto.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A4:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,54 +421,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Nombre</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>chino</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>PRODUCTO</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>CANTIDAD</t>
-        </is>
-      </c>
-    </row>
     <row r="4">
       <c r="A4" t="inlineStr">
-        <is>
-          <t>Zanahoria</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2.0</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>KG</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B4" t="inlineStr">
         <is>
           <t>$ 0.0</t>
         </is>

</xml_diff>